<commit_message>
Added Job Asset Verification In Property History
</commit_message>
<xml_diff>
--- a/TestData/MobileDatasheet.xlsx
+++ b/TestData/MobileDatasheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssara\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2f255e5693ee15f/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B9FFA0-0F8D-48F1-A546-936EED7B72D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{78B9FFA0-0F8D-48F1-A546-936EED7B72D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CD69879-CE20-4FEE-A8D7-968B3FF12DB8}"/>
   <bookViews>
-    <workbookView xWindow="4356" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{3FCEC922-A3B7-4FAC-BCE0-BCE5777AB953}"/>
+    <workbookView xWindow="2460" yWindow="1920" windowWidth="17280" windowHeight="9960" xr2:uid="{3FCEC922-A3B7-4FAC-BCE0-BCE5777AB953}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -128,6 +128,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -430,7 +434,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>